<commit_message>
Added configuration fro pom.xml
</commit_message>
<xml_diff>
--- a/target/classes/com/automationtesting/repo/TestData.xlsx
+++ b/target/classes/com/automationtesting/repo/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishnasakinala/Documents/workspace/POMWithPF/src/main/java/com/automationtesting/repo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krishnasakinala/hubiC/workspace/POMWPF_Framework/src/main/java/com/automationtesting/repo/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -409,7 +409,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>